<commit_message>
plotted all etnp flexes
</commit_message>
<xml_diff>
--- a/data/flux/2017_2018_flux+rate_MED.xlsx
+++ b/data/flux/2017_2018_flux+rate_MED.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="P2 Flux not control subtracted" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="RLS calc" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="P1" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="2018" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="rate calcs" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="200">
   <si>
     <t xml:space="preserve">P2</t>
   </si>
@@ -190,6 +191,9 @@
     <t xml:space="preserve">Keil 3-21</t>
   </si>
   <si>
+    <t xml:space="preserve">P1</t>
+  </si>
+  <si>
     <t xml:space="preserve">top collector: 600 mL</t>
   </si>
   <si>
@@ -259,9 +263,6 @@
     <t xml:space="preserve">fz0 is 1.29</t>
   </si>
   <si>
-    <t xml:space="preserve">P1</t>
-  </si>
-  <si>
     <t xml:space="preserve">mg org N/m2-d</t>
   </si>
   <si>
@@ -319,18 +320,322 @@
     <t xml:space="preserve">Time of OC accumulation</t>
   </si>
   <si>
+    <t xml:space="preserve">Org C flux (umol C/m2/day) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Org C flux mg org C/m2-d</t>
+  </si>
+  <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organic C fluxes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flux (mg/m2/day)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trap type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-30_151m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-30_151m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-31_121m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-31_121m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-32_147m_top_remainder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-32_147m_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-32_147m_+P_remainder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-32_147m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-32_147m_nw1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-32_147m_nw2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-32_147m_nw3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-32_147m_nw4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-33_368m_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-33_368m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-33_368m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-33_368m_nw1 (does this exist?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-33_368m_nw2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-33_368m_nw3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-33_586m_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-33_586m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-33_586m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-33_586m_nw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-34_87m_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-34_87m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-34_87m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-34_221m_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-34_221m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-34_221m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-36_85m_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-36_85m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-36_85m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-36_85m_nw1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-36_85m_nw2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-36_85m_nw3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-36_147m_nw1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-36_147m_nw2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-37_50m_+P1/top1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-37_50m_+P/top2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-37_50m_nw1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-37_50m_nw2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-37_120m_+P/top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-37_120m_nw1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-37_120m_nw2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-37_120m_nw3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-37_120m_nw4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-38_122m_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-38_122m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-38_122m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-39_120m_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-39_190m_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-39_190m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-39_190m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-40_123m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-40_123m_nw1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-40_123m_nw2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-40_123m_nw3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-40_201m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-40_201m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-40_201m_nw1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-40_201m_nw2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-40_201m_nw3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-40_201m_nw4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-40_201m_nw5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-42_221m_+P1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-42_221m_+P2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-42_221m_nw1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-42_221m_nw2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-42_221m_nw3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-42_221m_nw4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-42_586m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-42_586m_nw1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-42_586m_nw2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-42_586m_nw3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-42_586m_nw4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-43_145m_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-43_145m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-43_145m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-43_288m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-44_93m_top</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-44_93m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-44_93m_ctl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-45_143m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-45_143m_nw1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-45_143m_nw2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-45_143m_nw3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-45_143m_nw4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-45_143m_nw5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-45_843m_+P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-45_843m_nw1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-45_843m_nw2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-45_843m_nw3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-45_843m_nw4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N production rate (nM N/day)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organic C flux </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$-409]d\-mmm"/>
+    <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -420,12 +725,20 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -435,13 +748,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC4BD97"/>
-        <bgColor rgb="FFB3B3B3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
   </fills>
@@ -482,7 +789,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -503,7 +810,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -528,6 +843,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -557,7 +880,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFB3B3B3"/>
+      <rgbColor rgb="FFC4BD97"/>
       <rgbColor rgb="FF7F7F7F"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF7030A0"/>
@@ -582,13 +905,13 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFC4BD97"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF420E"/>
+      <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
@@ -604,7 +927,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -616,10 +939,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.10145979514477"/>
-          <c:y val="0.164468697892982"/>
-          <c:w val="0.85652068715219"/>
-          <c:h val="0.785356980445657"/>
+          <c:x val="0.101467978706243"/>
+          <c:y val="0.164481164253771"/>
+          <c:w val="0.856428456202613"/>
+          <c:h val="0.785264913211552"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -775,11 +1098,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="75121779"/>
-        <c:axId val="93023214"/>
+        <c:axId val="88712158"/>
+        <c:axId val="73599663"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="75121779"/>
+        <c:axId val="88712158"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -845,13 +1168,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93023214"/>
+        <c:crossAx val="73599663"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="93023214"/>
+        <c:axId val="73599663"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="1000"/>
@@ -884,7 +1207,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75121779"/>
+        <c:crossAx val="88712158"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -911,7 +1234,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -923,10 +1246,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.101480226820826"/>
-          <c:y val="0.164493026762156"/>
-          <c:w val="0.856469548567641"/>
-          <c:h val="0.785299660761402"/>
+          <c:x val="0.101487700692296"/>
+          <c:y val="0.164505428226779"/>
+          <c:w val="0.856385329209015"/>
+          <c:h val="0.785208082026538"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1078,11 +1401,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="41966885"/>
-        <c:axId val="16208391"/>
+        <c:axId val="69074976"/>
+        <c:axId val="28684446"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="41966885"/>
+        <c:axId val="69074976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1149,13 +1472,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16208391"/>
+        <c:crossAx val="28684446"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="16208391"/>
+        <c:axId val="28684446"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="300"/>
@@ -1188,7 +1511,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41966885"/>
+        <c:crossAx val="69074976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1215,7 +1538,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1227,10 +1550,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.206218774651591"/>
-          <c:y val="0.16439775081385"/>
-          <c:w val="0.73126479095451"/>
-          <c:h val="0.785365492749334"/>
+          <c:x val="0.206232331865098"/>
+          <c:y val="0.16440991490936"/>
+          <c:w val="0.731247123791993"/>
+          <c:h val="0.785275619681835"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1382,11 +1705,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1874869"/>
-        <c:axId val="24236978"/>
+        <c:axId val="39654700"/>
+        <c:axId val="20551887"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1874869"/>
+        <c:axId val="39654700"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -1454,12 +1777,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="24236978"/>
+        <c:crossAx val="20551887"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="24236978"/>
+        <c:axId val="20551887"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="1000"/>
@@ -1526,7 +1849,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1874869"/>
+        <c:crossAx val="39654700"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1553,7 +1876,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1565,10 +1888,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.206257934433575"/>
-          <c:y val="0.19674461582202"/>
-          <c:w val="0.731312075274438"/>
-          <c:h val="0.753003056365058"/>
+          <c:x val="0.206273338312173"/>
+          <c:y val="0.196758601080466"/>
+          <c:w val="0.731292008961912"/>
+          <c:h val="0.752914415695195"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1872,11 +2195,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="37015161"/>
-        <c:axId val="10932627"/>
+        <c:axId val="91083477"/>
+        <c:axId val="48984556"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="37015161"/>
+        <c:axId val="91083477"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -1914,8 +2237,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.170039578821597"/>
-              <c:y val="0.00525979102992395"/>
+              <c:x val="0.170126960418223"/>
+              <c:y val="0.00526016491327836"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1952,13 +2275,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10932627"/>
+        <c:crossAx val="48984556"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="10932627"/>
+        <c:axId val="48984556"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="300"/>
@@ -2025,7 +2348,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37015161"/>
+        <c:crossAx val="91083477"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2052,7 +2375,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2064,10 +2387,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.206261510128913"/>
-          <c:y val="0.164478536657324"/>
-          <c:w val="0.731307550644567"/>
-          <c:h val="0.785366573240891"/>
+          <c:x val="0.20627417275462"/>
+          <c:y val="0.164490669027071"/>
+          <c:w val="0.731291055313402"/>
+          <c:h val="0.785276978682599"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2078,7 +2401,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>"FLux"</c:f>
+              <c:f>label 1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2135,7 +2458,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'P2 Flux not control subtracted'!$P$3:$P$13</c:f>
+              <c:f>0</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2177,7 +2500,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'P2 Flux not control subtracted'!$Q$3:$Q$13</c:f>
+              <c:f>1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2219,11 +2542,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="25754701"/>
-        <c:axId val="83791684"/>
+        <c:axId val="708680"/>
+        <c:axId val="83440693"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="25754701"/>
+        <c:axId val="708680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -2291,12 +2614,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83791684"/>
+        <c:crossAx val="83440693"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="83791684"/>
+        <c:axId val="83440693"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="1000"/>
@@ -2363,7 +2686,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25754701"/>
+        <c:crossAx val="708680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2390,7 +2713,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2402,10 +2725,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.101490499487996"/>
-          <c:y val="0.164469347396177"/>
-          <c:w val="0.856525201956992"/>
-          <c:h val="0.785299934080422"/>
+          <c:x val="0.101496273539284"/>
+          <c:y val="0.164480189860901"/>
+          <c:w val="0.856460146782727"/>
+          <c:h val="0.785219856285846"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2546,11 +2869,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="65488482"/>
-        <c:axId val="18341432"/>
+        <c:axId val="68348182"/>
+        <c:axId val="17388416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="65488482"/>
+        <c:axId val="68348182"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2582,13 +2905,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18341432"/>
+        <c:crossAx val="17388416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="18341432"/>
+        <c:axId val="17388416"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="1000"/>
@@ -2621,7 +2944,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65488482"/>
+        <c:crossAx val="68348182"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="200"/>
@@ -2649,7 +2972,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2661,10 +2984,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.101522842639594"/>
-          <c:y val="0.164412568306011"/>
-          <c:w val="0.856488633855661"/>
-          <c:h val="0.785382513661202"/>
+          <c:x val="0.101528444518016"/>
+          <c:y val="0.164423799439852"/>
+          <c:w val="0.856425536610936"/>
+          <c:h val="0.785299542318464"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2962,11 +3285,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="25280481"/>
-        <c:axId val="33705648"/>
+        <c:axId val="18753577"/>
+        <c:axId val="24535336"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="25280481"/>
+        <c:axId val="18753577"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -2999,13 +3322,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33705648"/>
+        <c:crossAx val="24535336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="33705648"/>
+        <c:axId val="24535336"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="300"/>
@@ -3038,7 +3361,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25280481"/>
+        <c:crossAx val="18753577"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="50"/>
@@ -3066,7 +3389,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3078,10 +3401,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.206240212022648"/>
-          <c:y val="0.19681660899654"/>
-          <c:w val="0.731297434044091"/>
-          <c:h val="0.753010380622837"/>
+          <c:x val="0.206252635383411"/>
+          <c:y val="0.196830230465776"/>
+          <c:w val="0.731281248117583"/>
+          <c:h val="0.752924077790851"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3236,11 +3559,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="39720592"/>
-        <c:axId val="70388769"/>
+        <c:axId val="65033328"/>
+        <c:axId val="73699289"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="39720592"/>
+        <c:axId val="65033328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -3274,13 +3597,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70388769"/>
+        <c:crossAx val="73699289"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="70388769"/>
+        <c:axId val="73699289"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="300"/>
@@ -3313,7 +3636,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="39720592"/>
+        <c:crossAx val="65033328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3340,7 +3663,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart33.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3352,10 +3675,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.206237894877446"/>
-          <c:y val="0.164444781093774"/>
-          <c:w val="0.731316369465037"/>
-          <c:h val="0.785335555218906"/>
+          <c:x val="0.206251669783596"/>
+          <c:y val="0.164457238088024"/>
+          <c:w val="0.731298423724285"/>
+          <c:h val="0.785243542155897"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3366,7 +3689,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>"FLux"</c:f>
+              <c:f>label 1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3423,7 +3746,7 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>'P2 Flux not control subtracted'!$O$3:$O$13</c:f>
+              <c:f>0</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -3465,7 +3788,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'P2 Flux not control subtracted'!$Q$3:$Q$13</c:f>
+              <c:f>1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -3507,11 +3830,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="48968474"/>
-        <c:axId val="56929570"/>
+        <c:axId val="24972402"/>
+        <c:axId val="36981604"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="48968474"/>
+        <c:axId val="24972402"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3579,13 +3902,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56929570"/>
+        <c:crossAx val="36981604"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="56929570"/>
+        <c:axId val="36981604"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="1000"/>
@@ -3652,7 +3975,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48968474"/>
+        <c:crossAx val="24972402"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3679,7 +4002,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart34.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3691,10 +4014,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.206266318537859"/>
-          <c:y val="0.196755994358251"/>
-          <c:w val="0.731319159517593"/>
-          <c:h val="0.75296191819464"/>
+          <c:x val="0.206279142057818"/>
+          <c:y val="0.196769870935891"/>
+          <c:w val="0.731302455704072"/>
+          <c:h val="0.752873968545031"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3921,11 +4244,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="40683306"/>
-        <c:axId val="60545066"/>
+        <c:axId val="51553277"/>
+        <c:axId val="90449933"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="40683306"/>
+        <c:axId val="51553277"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -3959,13 +4282,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60545066"/>
+        <c:crossAx val="90449933"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="60545066"/>
+        <c:axId val="90449933"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="300"/>
@@ -3998,7 +4321,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40683306"/>
+        <c:crossAx val="51553277"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4025,7 +4348,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart35.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4037,10 +4360,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.101533197341581"/>
-          <c:y val="0.164399179144182"/>
-          <c:w val="0.856484832532737"/>
-          <c:h val="0.785361404575511"/>
+          <c:x val="0.101539878915504"/>
+          <c:y val="0.164411675281241"/>
+          <c:w val="0.856409581468808"/>
+          <c:h val="0.78526907874734"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -4184,11 +4507,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="96567995"/>
-        <c:axId val="90693581"/>
+        <c:axId val="83753133"/>
+        <c:axId val="41325808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="96567995"/>
+        <c:axId val="83753133"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -4225,8 +4548,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.23234848983352"/>
-              <c:y val="0.0241696435357604"/>
+              <c:x val="0.23236377994209"/>
+              <c:y val="0.024247491638796"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -4263,13 +4586,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="90693581"/>
+        <c:crossAx val="41325808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="90693581"/>
+        <c:axId val="41325808"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="700"/>
@@ -4302,7 +4625,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96567995"/>
+        <c:crossAx val="83753133"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4329,280 +4652,20 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'2018'!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Sediment trap rate nM/d</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ff420e"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="diamond"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr wrap="none"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:separator> </c:separator>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'2018'!$B$2:$B$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>93</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>122</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>190</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'2018'!$D$2:$D$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>54</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>181</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>64</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:axId val="91176904"/>
-        <c:axId val="59063862"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="91176904"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>N loss [ nM N/day]</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="59063862"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="59063862"/>
-        <c:scaling>
-          <c:orientation val="maxMin"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="0">
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln w="0">
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="91176904"/>
-        <c:crossesAt val="0"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-              <a:latin typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="span"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln w="0">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>648720</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:colOff>660240</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>74520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>432000</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>177840</xdr:rowOff>
+      <xdr:colOff>443160</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>61200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4610,8 +4673,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1668240" y="2857680"/>
-        <a:ext cx="4463280" cy="4749480"/>
+        <a:off x="1679760" y="4836960"/>
+        <a:ext cx="4462920" cy="4749120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4624,15 +4687,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>743760</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:colOff>831960</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>43200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>545400</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>12960</xdr:rowOff>
+      <xdr:colOff>633240</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>55440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4640,8 +4703,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6443280" y="2857680"/>
-        <a:ext cx="4888080" cy="4775040"/>
+        <a:off x="6531480" y="5376960"/>
+        <a:ext cx="4887720" cy="4774680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4653,16 +4716,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>571680</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>103320</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>43200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>619560</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>103320</xdr:rowOff>
+      <xdr:colOff>1674000</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>145800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4670,8 +4733,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11357640" y="2857680"/>
-        <a:ext cx="5475960" cy="4865400"/>
+        <a:off x="12412440" y="5376960"/>
+        <a:ext cx="5475600" cy="4865040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4683,16 +4746,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>775080</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>412200</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>720</xdr:rowOff>
+      <xdr:rowOff>149040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>932040</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>111960</xdr:rowOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>359280</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>69480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4700,8 +4763,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="38612160" y="3048480"/>
-        <a:ext cx="4820400" cy="5064480"/>
+        <a:off x="41099040" y="3196800"/>
+        <a:ext cx="4820040" cy="5064120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4714,15 +4777,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>1051200</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:colOff>1379880</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>354600</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>118440</xdr:rowOff>
+      <xdr:colOff>578880</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>1800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4730,8 +4793,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="17265240" y="2857680"/>
-        <a:ext cx="5864040" cy="4880520"/>
+        <a:off x="17593920" y="5334480"/>
+        <a:ext cx="5759640" cy="3239640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4744,7 +4807,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>7200</xdr:colOff>
+      <xdr:colOff>7560</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -4752,7 +4815,7 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>635040</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>127080</xdr:rowOff>
+      <xdr:rowOff>126720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4760,8 +4823,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2046600" y="8191440"/>
-        <a:ext cx="6327720" cy="5460840"/>
+        <a:off x="2046960" y="8191440"/>
+        <a:ext cx="6327360" cy="5460480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4780,9 +4843,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>139680</xdr:colOff>
+      <xdr:colOff>139320</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>126720</xdr:rowOff>
+      <xdr:rowOff>126360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4791,7 +4854,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="8711640" y="8381880"/>
-        <a:ext cx="6524280" cy="5270040"/>
+        <a:ext cx="6523920" cy="5269680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4804,9 +4867,9 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>718560</xdr:colOff>
+      <xdr:colOff>718920</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>360</xdr:rowOff>
+      <xdr:rowOff>720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>36</xdr:col>
@@ -4820,8 +4883,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="44238600" y="2857680"/>
-        <a:ext cx="5976360" cy="5201640"/>
+        <a:off x="44238960" y="2858040"/>
+        <a:ext cx="5976000" cy="5201280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4840,9 +4903,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>1016280</xdr:colOff>
+      <xdr:colOff>1015920</xdr:colOff>
       <xdr:row>68</xdr:row>
-      <xdr:rowOff>180360</xdr:rowOff>
+      <xdr:rowOff>180000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4851,7 +4914,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="16214040" y="8381880"/>
-        <a:ext cx="5389920" cy="4752360"/>
+        <a:ext cx="5389560" cy="4752000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4864,7 +4927,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>360</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>177840</xdr:rowOff>
     </xdr:from>
@@ -4872,7 +4935,7 @@
       <xdr:col>42</xdr:col>
       <xdr:colOff>691560</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>138960</xdr:rowOff>
+      <xdr:rowOff>138600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4880,8 +4943,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="50658840" y="2844720"/>
-        <a:ext cx="5790600" cy="5104440"/>
+        <a:off x="50659200" y="2844720"/>
+        <a:ext cx="5790240" cy="5104080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4905,9 +4968,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>138960</xdr:colOff>
+      <xdr:colOff>138600</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>164880</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4916,42 +4979,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="3846600" y="3048480"/>
-        <a:ext cx="5470560" cy="4736160"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>476280</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>122040</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>550080</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>58320</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame>
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="11" name=""/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="5352840" y="447120"/>
-        <a:ext cx="5763600" cy="3243240"/>
+        <a:ext cx="5470200" cy="4735800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4969,13 +4997,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BL32"/>
+  <dimension ref="A1:BL40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Y1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB3" activeCellId="0" sqref="AB3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N3" activeCellId="0" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="10.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.67"/>
@@ -5208,6 +5236,12 @@
         <f aca="false">N3/$AD$2</f>
         <v>0.651632371191503</v>
       </c>
+      <c r="W3" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="X3" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="Y3" s="0" t="n">
         <v>100</v>
       </c>
@@ -5293,6 +5327,12 @@
         <f aca="false">N4/$AD$2</f>
         <v>0.153050454961832</v>
       </c>
+      <c r="W4" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="X4" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="Y4" s="0" t="n">
         <v>100</v>
       </c>
@@ -5377,6 +5417,12 @@
       <c r="U5" s="0" t="n">
         <f aca="false">N5/$AD$2</f>
         <v>0.117400681314305</v>
+      </c>
+      <c r="W5" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="X5" s="0" t="s">
+        <v>0</v>
       </c>
       <c r="Y5" s="0" t="n">
         <v>100</v>
@@ -5462,6 +5508,12 @@
         <f aca="false">N6/$AD$2</f>
         <v>0.155434020577497</v>
       </c>
+      <c r="W6" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="X6" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="Y6" s="0" t="n">
         <v>113</v>
       </c>
@@ -5554,6 +5606,12 @@
         <f aca="false">N7/$AD$2</f>
         <v>0.0430258344442376</v>
       </c>
+      <c r="W7" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="X7" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="Y7" s="0" t="n">
         <v>120</v>
       </c>
@@ -5646,6 +5704,12 @@
         <f aca="false">N8/$AD$2</f>
         <v>0.0759534858280783</v>
       </c>
+      <c r="W8" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="X8" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="Y8" s="0" t="n">
         <v>120</v>
       </c>
@@ -5738,6 +5802,12 @@
         <f aca="false">N9/$AD$2</f>
         <v>0.0586321683113014</v>
       </c>
+      <c r="W9" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="X9" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="Y9" s="0" t="n">
         <v>140</v>
       </c>
@@ -5825,6 +5895,12 @@
         <f aca="false">N10/$AD$2</f>
         <v>0.0561179373182394</v>
       </c>
+      <c r="W10" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="X10" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="Y10" s="0" t="n">
         <v>150</v>
       </c>
@@ -5899,15 +5975,25 @@
         <f aca="false">N11/12</f>
         <v>0.0356523414634146</v>
       </c>
-      <c r="S11" s="4"/>
-      <c r="T11" s="4"/>
+      <c r="S11" s="0" t="n">
+        <f aca="false">(H11/1000)/F11</f>
+        <v>0.70163808</v>
+      </c>
+      <c r="T11" s="0" t="n">
+        <f aca="false">(S11/12)*1000</f>
+        <v>58.46984</v>
+      </c>
       <c r="U11" s="4" t="n">
         <f aca="false">N11/$AD$2</f>
         <v>0.0506208817724819</v>
       </c>
       <c r="V11" s="4"/>
-      <c r="W11" s="4"/>
-      <c r="X11" s="4"/>
+      <c r="W11" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="X11" s="0" t="s">
+        <v>0</v>
+      </c>
       <c r="Y11" s="4" t="n">
         <v>150</v>
       </c>
@@ -6018,21 +6104,31 @@
         <f aca="false">N12/12</f>
         <v>0.0528342341463415</v>
       </c>
-      <c r="S12" s="4"/>
-      <c r="T12" s="4"/>
+      <c r="S12" s="0" t="n">
+        <f aca="false">(H12/1000)/F12</f>
+        <v>1.039777728</v>
+      </c>
+      <c r="T12" s="0" t="n">
+        <f aca="false">(S12/12)*1000</f>
+        <v>86.648144</v>
+      </c>
       <c r="U12" s="4" t="n">
         <f aca="false">N12/$AD$2</f>
         <v>0.0750165461925154</v>
       </c>
       <c r="V12" s="4"/>
-      <c r="W12" s="4"/>
-      <c r="X12" s="4"/>
-      <c r="Y12" s="4" t="n">
+      <c r="W12" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="X12" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="5" t="n">
         <v>150</v>
       </c>
-      <c r="Z12" s="4"/>
-      <c r="AA12" s="4"/>
-      <c r="AB12" s="4" t="n">
+      <c r="Z12" s="5"/>
+      <c r="AA12" s="5"/>
+      <c r="AB12" s="5" t="n">
         <v>16</v>
       </c>
       <c r="AC12" s="4"/>
@@ -6137,128 +6233,503 @@
         <f aca="false">(H13/1000)/F13</f>
         <v>0.52786602</v>
       </c>
-      <c r="Y13" s="5" t="n">
+      <c r="T13" s="0" t="n">
+        <f aca="false">(S13/12)*1000</f>
+        <v>43.988835</v>
+      </c>
+      <c r="U13" s="4" t="n">
+        <f aca="false">N13/$AD$2</f>
+        <v>0.0214273680526883</v>
+      </c>
+      <c r="W13" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="X13" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="6" t="n">
         <v>179</v>
       </c>
-      <c r="Z13" s="5" t="n">
+      <c r="Z13" s="6" t="n">
         <v>31</v>
       </c>
-      <c r="AA13" s="5" t="n">
+      <c r="AA13" s="6" t="n">
         <f aca="false">Z13/S9</f>
         <v>33.2905400742214</v>
       </c>
-      <c r="AB13" s="5" t="n">
+      <c r="AB13" s="6" t="n">
         <f aca="false">AA13*U9</f>
         <v>1.95189654880588</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Y14" s="5" t="n">
+      <c r="A14" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <v>0.35039640768</v>
+      </c>
+      <c r="R14" s="0" t="n">
+        <f aca="false">N14/12</f>
+        <v>0.02919970064</v>
+      </c>
+      <c r="U14" s="4" t="n">
+        <f aca="false">N14/$AD$2</f>
+        <v>0.0414591169392366</v>
+      </c>
+      <c r="W14" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="X14" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="6" t="n">
         <v>180</v>
       </c>
-      <c r="Z14" s="5" t="n">
+      <c r="Z14" s="6" t="n">
         <v>39</v>
       </c>
-      <c r="AA14" s="5" t="n">
+      <c r="AA14" s="6" t="n">
         <f aca="false">Z14/S9</f>
         <v>41.8816471901496</v>
       </c>
-      <c r="AB14" s="5" t="n">
+      <c r="AB14" s="6" t="n">
         <f aca="false">AA14*U9</f>
         <v>2.45561178720739</v>
       </c>
     </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>122</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <v>0.58685784336</v>
+      </c>
+      <c r="R15" s="0" t="n">
+        <f aca="false">N15/12</f>
+        <v>0.04890482028</v>
+      </c>
+      <c r="U15" s="4" t="n">
+        <f aca="false">N15/$AD$2</f>
+        <v>0.0694373784128244</v>
+      </c>
+      <c r="W15" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="X15" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y15" s="6" t="n">
+        <v>93</v>
+      </c>
+      <c r="Z15" s="6" t="n">
+        <v>160</v>
+      </c>
+      <c r="AA15" s="6"/>
+      <c r="AB15" s="7" t="n">
+        <f aca="false">AA15*U10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>145</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <v>0.24311220636</v>
+      </c>
+      <c r="R16" s="0" t="n">
+        <f aca="false">N16/12</f>
+        <v>0.02025935053</v>
+      </c>
+      <c r="U16" s="4" t="n">
+        <f aca="false">N16/$AD$2</f>
+        <v>0.0287651847219847</v>
+      </c>
+      <c r="W16" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="X16" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y16" s="6" t="n">
+        <v>122</v>
+      </c>
+      <c r="Z16" s="6" t="n">
+        <v>54</v>
+      </c>
+      <c r="AA16" s="6"/>
+      <c r="AB16" s="7" t="n">
+        <f aca="false">AA16*U11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>190</v>
+      </c>
+      <c r="N17" s="0" t="n">
+        <v>0.2981113254</v>
+      </c>
+      <c r="R17" s="0" t="n">
+        <f aca="false">N17/12</f>
+        <v>0.02484261045</v>
+      </c>
+      <c r="U17" s="4" t="n">
+        <f aca="false">N17/$AD$2</f>
+        <v>0.0352727140740458</v>
+      </c>
+      <c r="W17" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="X17" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y17" s="6" t="n">
+        <v>145</v>
+      </c>
+      <c r="Z17" s="6" t="n">
+        <v>181</v>
+      </c>
+      <c r="AA17" s="6"/>
+      <c r="AB17" s="7" t="n">
+        <f aca="false">AA17*U12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="N18" s="0" t="n">
+        <v>1.3821818328</v>
+      </c>
+      <c r="R18" s="0" t="n">
+        <f aca="false">N18/12</f>
+        <v>0.1151818194</v>
+      </c>
+      <c r="U18" s="4" t="n">
+        <f aca="false">N18/$AD$2</f>
+        <v>0.163540598537405</v>
+      </c>
+      <c r="W18" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="X18" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y18" s="6" t="n">
+        <v>190</v>
+      </c>
+      <c r="Z18" s="6" t="n">
+        <v>64</v>
+      </c>
+      <c r="AA18" s="6"/>
+      <c r="AB18" s="7" t="n">
+        <f aca="false">AA18*U13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="N19" s="0" t="n">
+        <v>0.65778210996</v>
+      </c>
+      <c r="R19" s="0" t="n">
+        <f aca="false">N19/12</f>
+        <v>0.05481517583</v>
+      </c>
+      <c r="U19" s="4" t="n">
+        <f aca="false">N19/$AD$2</f>
+        <v>0.0778291809494656</v>
+      </c>
+      <c r="W19" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="X19" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="6" t="n">
+        <v>85</v>
+      </c>
+      <c r="Z19" s="6" t="n">
+        <v>530</v>
+      </c>
+      <c r="AA19" s="6"/>
+      <c r="AB19" s="7" t="n">
+        <f aca="false">AA19*U14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="N20" s="0" t="n">
+        <v>1.7063034312</v>
+      </c>
+      <c r="R20" s="0" t="n">
+        <f aca="false">N20/12</f>
+        <v>0.1421919526</v>
+      </c>
+      <c r="U20" s="4" t="n">
+        <f aca="false">N20/$AD$2</f>
+        <v>0.201890863996947</v>
+      </c>
+      <c r="W20" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="X20" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="6" t="n">
+        <v>87</v>
+      </c>
+      <c r="Z20" s="6" t="n">
+        <v>38.5</v>
+      </c>
+      <c r="AA20" s="6"/>
+      <c r="AB20" s="7" t="n">
+        <f aca="false">AA20*U15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="N21" s="0" t="n">
+        <v>0.073060043712</v>
+      </c>
+      <c r="R21" s="0" t="n">
+        <f aca="false">N21/12</f>
+        <v>0.006088336976</v>
+      </c>
+      <c r="U21" s="4" t="n">
+        <f aca="false">N21/$AD$2</f>
+        <v>0.00864450898882443</v>
+      </c>
+      <c r="W21" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="X21" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="6" t="n">
+        <v>120</v>
+      </c>
+      <c r="Z21" s="6"/>
+      <c r="AA21" s="6"/>
+      <c r="AB21" s="7" t="n">
+        <f aca="false">AA21*U16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>221</v>
+      </c>
+      <c r="R22" s="0" t="n">
+        <f aca="false">N22/12</f>
+        <v>0</v>
+      </c>
+      <c r="U22" s="4" t="n">
+        <f aca="false">N22/$AD$2</f>
+        <v>0</v>
+      </c>
+      <c r="W22" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="X22" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="6" t="n">
+        <v>150</v>
+      </c>
+      <c r="Z22" s="6" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA22" s="6"/>
+      <c r="AB22" s="7" t="n">
+        <f aca="false">AA22*U17</f>
+        <v>0</v>
+      </c>
+    </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S23" s="0" t="s">
-        <v>55</v>
+      <c r="A23" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>368</v>
+      </c>
+      <c r="N23" s="0" t="n">
+        <v>0.44133636708</v>
+      </c>
+      <c r="R23" s="0" t="n">
+        <f aca="false">N23/12</f>
+        <v>0.03677803059</v>
+      </c>
+      <c r="U23" s="4" t="n">
+        <f aca="false">N23/$AD$2</f>
+        <v>0.0522191884712977</v>
+      </c>
+      <c r="W23" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="X23" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="6" t="n">
+        <v>221</v>
+      </c>
+      <c r="Z23" s="6" t="n">
+        <v>13</v>
+      </c>
+      <c r="AA23" s="6"/>
+      <c r="AB23" s="7" t="n">
+        <f aca="false">AA23*U18</f>
+        <v>0</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S24" s="0" t="s">
+      <c r="W24" s="0" t="n">
+        <v>2018</v>
+      </c>
+      <c r="X24" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="6" t="n">
+        <v>368</v>
+      </c>
+      <c r="Z24" s="6" t="n">
+        <v>375</v>
+      </c>
+      <c r="AA24" s="6"/>
+      <c r="AB24" s="7" t="n">
+        <f aca="false">AA24*U19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S31" s="0" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S25" s="0" t="s">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S32" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="T25" s="0" t="s">
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S33" s="0" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S26" s="0" t="s">
+      <c r="T33" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="T26" s="0" t="s">
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S34" s="0" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="W27" s="0" t="s">
+      <c r="T34" s="0" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S28" s="0" t="s">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="W35" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="T28" s="0" t="s">
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S36" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="U28" s="0" t="s">
+      <c r="T36" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="V28" s="0" t="s">
+      <c r="U36" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="W28" s="0" t="n">
+      <c r="V36" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="W36" s="0" t="n">
         <f aca="false">PI()*(21/2)^2</f>
         <v>346.360590058275</v>
       </c>
-      <c r="X28" s="0" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="S29" s="0" t="s">
+      <c r="X36" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="T29" s="0" t="s">
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="S37" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="U29" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="W29" s="0" t="n">
+      <c r="T37" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="U37" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="W37" s="0" t="n">
         <f aca="false">(PI()*(38.1/2)^2)</f>
         <v>1140.09182796937</v>
       </c>
-      <c r="X29" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y29" s="0" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Y30" s="0" t="n">
-        <f aca="false">W28*(1-0.064)</f>
+      <c r="X37" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y37" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y38" s="0" t="n">
+        <f aca="false">W36*(1-0.064)</f>
         <v>324.193512294545</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="W31" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="X31" s="0" t="n">
-        <f aca="false">W29/Y30</f>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="W39" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="X39" s="0" t="n">
+        <f aca="false">W37/Y38</f>
         <v>3.51670155241584</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="W32" s="0" t="s">
-        <v>71</v>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="W40" s="0" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -6284,34 +6755,34 @@
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.66"/>
   </cols>
   <sheetData>
-    <row r="1" s="7" customFormat="true" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" s="7" t="s">
+    <row r="1" s="9" customFormat="true" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>73</v>
       </c>
+      <c r="C1" s="9" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="A2" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>75</v>
+      <c r="C2" s="8" t="s">
+        <v>76</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>100</v>
@@ -6329,7 +6800,7 @@
         <v>21.3983044092961</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>1.2935232</v>
@@ -6461,11 +6932,11 @@
   </sheetPr>
   <dimension ref="A1:S17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M8" activeCellId="0" sqref="M8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="1" style="0" width="10.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="16.84"/>
@@ -6479,7 +6950,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>6</v>
@@ -6512,7 +6983,7 @@
         <v>7</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="R1" s="0" t="s">
         <v>7</v>
@@ -6599,10 +7070,10 @@
       <c r="G3" s="0" t="n">
         <v>0.6</v>
       </c>
-      <c r="H3" s="8" t="n">
+      <c r="H3" s="10" t="n">
         <v>12</v>
       </c>
-      <c r="I3" s="9" t="n">
+      <c r="I3" s="11" t="n">
         <v>103.2737</v>
       </c>
       <c r="J3" s="0" t="n">
@@ -6643,21 +7114,21 @@
       <c r="G4" s="4" t="n">
         <v>1.6</v>
       </c>
-      <c r="H4" s="8" t="n">
+      <c r="H4" s="10" t="n">
         <v>32</v>
       </c>
-      <c r="I4" s="10" t="n">
+      <c r="I4" s="12" t="n">
         <v>142.7073</v>
       </c>
       <c r="J4" s="0" t="n">
         <f aca="false">I4*3.52</f>
         <v>502.329696</v>
       </c>
-      <c r="K4" s="10" t="n">
+      <c r="K4" s="12" t="n">
         <v>111.2036</v>
       </c>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
       <c r="N4" s="0" t="n">
         <f aca="false">(J4/1000)/(E4*(H4/24))</f>
         <v>0.819015808695652</v>
@@ -6695,7 +7166,7 @@
       <c r="H5" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="I5" s="9" t="n">
+      <c r="I5" s="11" t="n">
         <v>56.6686</v>
       </c>
       <c r="J5" s="0" t="n">
@@ -6739,7 +7210,7 @@
       <c r="H6" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="I6" s="9" t="n">
+      <c r="I6" s="11" t="n">
         <v>77.1038</v>
       </c>
       <c r="J6" s="0" t="n">
@@ -6783,7 +7254,7 @@
       <c r="H7" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="I7" s="9" t="n">
+      <c r="I7" s="11" t="n">
         <v>72.3089</v>
       </c>
       <c r="J7" s="0" t="n">
@@ -6824,17 +7295,17 @@
       <c r="G8" s="0" t="n">
         <v>0.6</v>
       </c>
-      <c r="H8" s="11" t="n">
+      <c r="H8" s="13" t="n">
         <v>24</v>
       </c>
-      <c r="I8" s="9" t="n">
+      <c r="I8" s="11" t="n">
         <v>275.9063</v>
       </c>
       <c r="J8" s="0" t="n">
         <f aca="false">I8*3.52</f>
         <v>971.190176</v>
       </c>
-      <c r="L8" s="9" t="n">
+      <c r="L8" s="11" t="n">
         <v>54.3155</v>
       </c>
       <c r="M8" s="0" t="n">
@@ -6886,7 +7357,7 @@
       <c r="H9" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="I9" s="9" t="n">
+      <c r="I9" s="11" t="n">
         <v>149.5976</v>
       </c>
       <c r="J9" s="0" t="n">
@@ -6932,7 +7403,7 @@
       <c r="H10" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="I10" s="9" t="n">
+      <c r="I10" s="11" t="n">
         <v>88.8127</v>
       </c>
       <c r="J10" s="0" t="n">
@@ -6978,14 +7449,14 @@
       <c r="H11" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="I11" s="9" t="n">
+      <c r="I11" s="11" t="n">
         <v>175.4337</v>
       </c>
       <c r="J11" s="0" t="n">
         <f aca="false">I11*3.52</f>
         <v>617.526624</v>
       </c>
-      <c r="L11" s="9" t="n">
+      <c r="L11" s="11" t="n">
         <v>27.7126</v>
       </c>
       <c r="M11" s="0" t="n">
@@ -7037,14 +7508,14 @@
       <c r="H12" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="I12" s="9" t="n">
+      <c r="I12" s="11" t="n">
         <v>418.4212</v>
       </c>
       <c r="J12" s="0" t="n">
         <f aca="false">I12*3.52</f>
         <v>1472.842624</v>
       </c>
-      <c r="L12" s="9" t="n">
+      <c r="L12" s="11" t="n">
         <v>49.3413</v>
       </c>
       <c r="M12" s="0" t="n">
@@ -7096,17 +7567,17 @@
       <c r="H13" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="I13" s="9" t="n">
+      <c r="I13" s="11" t="n">
         <v>224.1651</v>
       </c>
       <c r="J13" s="0" t="n">
         <f aca="false">I13*3.52</f>
         <v>789.061152</v>
       </c>
-      <c r="K13" s="10" t="n">
+      <c r="K13" s="12" t="n">
         <v>71.9624</v>
       </c>
-      <c r="L13" s="9" t="n">
+      <c r="L13" s="11" t="n">
         <v>28.1653</v>
       </c>
       <c r="M13" s="0" t="n">
@@ -7159,15 +7630,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB13"/>
+  <dimension ref="A1:AB109"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.3671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>94</v>
       </c>
@@ -7183,10 +7654,16 @@
       <c r="E1" s="0" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>93</v>
@@ -7200,10 +7677,17 @@
       <c r="E2" s="0" t="n">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F2" s="0" t="n">
+        <v>29.19970064</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <f aca="false">F2*12/1000</f>
+        <v>0.35039640768</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>122</v>
@@ -7217,13 +7701,20 @@
       <c r="E3" s="0" t="n">
         <v>20</v>
       </c>
+      <c r="F3" s="0" t="n">
+        <v>48.90482028</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <f aca="false">F3*12/1000</f>
+        <v>0.58685784336</v>
+      </c>
       <c r="AB3" s="0" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>145</v>
@@ -7237,10 +7728,17 @@
       <c r="E4" s="0" t="n">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F4" s="0" t="n">
+        <v>20.25935053</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <f aca="false">F4*12/1000</f>
+        <v>0.24311220636</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>190</v>
@@ -7253,6 +7751,13 @@
       </c>
       <c r="E5" s="0" t="n">
         <v>20</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>24.84261045</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <f aca="false">F5*12/1000</f>
+        <v>0.2981113254</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -7273,7 +7778,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>0</v>
       </c>
@@ -7289,8 +7794,15 @@
       <c r="E8" s="0" t="n">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F8" s="0" t="n">
+        <v>115.1818194</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <f aca="false">F8*12/1000</f>
+        <v>1.3821818328</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>0</v>
       </c>
@@ -7306,8 +7818,15 @@
       <c r="E9" s="0" t="n">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F9" s="0" t="n">
+        <v>54.81517583</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <f aca="false">F9*12/1000</f>
+        <v>0.65778210996</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>0</v>
       </c>
@@ -7320,8 +7839,15 @@
       <c r="E10" s="0" t="n">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F10" s="0" t="n">
+        <v>142.1919526</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <f aca="false">F10*12/1000</f>
+        <v>1.7063034312</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>0</v>
       </c>
@@ -7337,8 +7863,15 @@
       <c r="E11" s="0" t="n">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F11" s="0" t="n">
+        <v>6.088336976</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <f aca="false">F11*12/1000</f>
+        <v>0.073060043712</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>0</v>
       </c>
@@ -7355,7 +7888,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>0</v>
       </c>
@@ -7370,6 +7903,1227 @@
       </c>
       <c r="E13" s="0" t="n">
         <v>50</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>36.77803059</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <f aca="false">F13*12/1000</f>
+        <v>0.44133636708</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>151</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>59.93179319</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>114.4817664</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>151</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>121</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>140.2346446</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <v>142.1919526</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>121</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>135.5691057</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <v>6.088336976</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>368</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>5.577733349</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <v>36.77803059</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>586</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>8.164440297</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>49.69913676</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>24.18012422</v>
+      </c>
+      <c r="F40" s="0" t="n">
+        <v>54.81517583</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="G41" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="G42" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>221</v>
+      </c>
+      <c r="G43" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="G44" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="G45" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <v>26.58868425</v>
+      </c>
+      <c r="F46" s="0" t="n">
+        <v>115.1818194</v>
+      </c>
+      <c r="G46" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="G47" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="G48" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="G49" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="G50" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="G51" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="G52" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="G53" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="F54" s="0" t="n">
+        <v>244.4055742</v>
+      </c>
+      <c r="G54" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G55" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G56" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G57" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="G58" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G59" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G60" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G61" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G62" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D63" s="0" t="n">
+        <v>122</v>
+      </c>
+      <c r="E63" s="0" t="n">
+        <v>32.66219522</v>
+      </c>
+      <c r="F63" s="0" t="n">
+        <v>48.90482028</v>
+      </c>
+      <c r="G63" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G64" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G65" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D66" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="E66" s="0" t="n">
+        <v>144.5962733</v>
+      </c>
+      <c r="F66" s="0" t="n">
+        <v>47.19008443</v>
+      </c>
+      <c r="G66" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D67" s="0" t="n">
+        <v>190</v>
+      </c>
+      <c r="E67" s="0" t="n">
+        <v>31.86596927</v>
+      </c>
+      <c r="F67" s="0" t="n">
+        <v>24.84261045</v>
+      </c>
+      <c r="G67" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G68" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G69" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D70" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="E70" s="0" t="n">
+        <v>127.6422764</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="C71" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D74" s="0" t="n">
+        <v>201</v>
+      </c>
+      <c r="E74" s="0" t="n">
+        <v>18.53988134</v>
+      </c>
+      <c r="F74" s="0" t="n">
+        <v>206.4532045</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D81" s="0" t="n">
+        <v>221</v>
+      </c>
+      <c r="G81" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E82" s="0" t="n">
+        <v>7.360697997</v>
+      </c>
+      <c r="F82" s="0" t="n">
+        <v>94.40429427</v>
+      </c>
+      <c r="G82" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G83" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G84" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G85" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="C86" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G86" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="C87" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D87" s="0" t="n">
+        <v>586</v>
+      </c>
+      <c r="E87" s="0" t="n">
+        <v>5.35131205</v>
+      </c>
+      <c r="F87" s="0" t="n">
+        <v>54.4451539</v>
+      </c>
+      <c r="G87" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="C88" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G88" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="C89" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G89" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="C90" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G90" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="C91" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G91" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="C92" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D92" s="0" t="n">
+        <v>145</v>
+      </c>
+      <c r="E92" s="0" t="n">
+        <v>16.09712027</v>
+      </c>
+      <c r="F92" s="0" t="n">
+        <v>20.25935053</v>
+      </c>
+      <c r="G92" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="C93" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G93" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>182</v>
+      </c>
+      <c r="C94" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G94" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="C95" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D95" s="0" t="n">
+        <v>288</v>
+      </c>
+      <c r="E95" s="0" t="n">
+        <v>9.216589862</v>
+      </c>
+      <c r="F95" s="0" t="n">
+        <v>113.4440422</v>
+      </c>
+      <c r="G95" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="C96" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D96" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="E96" s="0" t="n">
+        <v>13.12777285</v>
+      </c>
+      <c r="F96" s="0" t="n">
+        <v>29.19970064</v>
+      </c>
+      <c r="G96" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="C97" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G97" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="C98" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G98" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="C99" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D99" s="0" t="n">
+        <v>143</v>
+      </c>
+      <c r="E99" s="0" t="n">
+        <v>54.63414634</v>
+      </c>
+      <c r="F99" s="0" t="n">
+        <v>44.60837344</v>
+      </c>
+      <c r="G99" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="C100" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G100" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="C101" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G101" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="C102" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G102" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="C103" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G103" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="C104" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G104" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="C105" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="D105" s="0" t="n">
+        <v>843</v>
+      </c>
+      <c r="F105" s="0" t="n">
+        <v>28.51596639</v>
+      </c>
+      <c r="G105" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="C106" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G106" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="C107" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G107" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
+        <v>196</v>
+      </c>
+      <c r="C108" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G108" s="0" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="C109" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="G109" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -7380,6 +9134,412 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.3671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1016" min="1" style="15" width="8.36"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="15" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="15" t="n">
+        <v>100</v>
+      </c>
+      <c r="D2" s="15" t="n">
+        <v>15</v>
+      </c>
+      <c r="E2" s="15" t="n">
+        <v>5.50734455652174</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="15" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="15" t="n">
+        <v>100</v>
+      </c>
+      <c r="D3" s="15" t="n">
+        <v>29</v>
+      </c>
+      <c r="E3" s="15" t="n">
+        <v>1.2935232</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="15" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="15" t="n">
+        <v>100</v>
+      </c>
+      <c r="E4" s="15" t="n">
+        <v>0.992225113043478</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="15" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="15" t="n">
+        <v>113</v>
+      </c>
+      <c r="D5" s="15" t="n">
+        <v>34</v>
+      </c>
+      <c r="E5" s="15" t="n">
+        <v>1.31366817391304</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="15" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="15" t="n">
+        <v>120</v>
+      </c>
+      <c r="D6" s="15" t="n">
+        <v>16</v>
+      </c>
+      <c r="E6" s="15" t="n">
+        <v>0.363637697560976</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="15" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="15" t="n">
+        <v>120</v>
+      </c>
+      <c r="D7" s="15" t="n">
+        <v>21</v>
+      </c>
+      <c r="E7" s="15" t="n">
+        <v>0.641929460869565</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="15" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="15" t="n">
+        <v>140</v>
+      </c>
+      <c r="D8" s="15" t="n">
+        <v>10</v>
+      </c>
+      <c r="E8" s="15" t="n">
+        <v>0.495536390243902</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="15" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="15" t="n">
+        <v>150</v>
+      </c>
+      <c r="D9" s="15" t="n">
+        <v>30</v>
+      </c>
+      <c r="E9" s="15" t="n">
+        <v>0.474287083141249</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="15" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="15" t="n">
+        <v>150</v>
+      </c>
+      <c r="D10" s="15" t="n">
+        <v>24</v>
+      </c>
+      <c r="E10" s="15" t="n">
+        <v>0.427828097560976</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="15" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="15" t="n">
+        <v>150</v>
+      </c>
+      <c r="E11" s="15" t="n">
+        <v>0.634010809756098</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="15" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="15" t="n">
+        <v>179</v>
+      </c>
+      <c r="D12" s="15" t="n">
+        <v>31</v>
+      </c>
+      <c r="E12" s="15" t="n">
+        <v>0.181095820316269</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="15" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="15" t="n">
+        <v>180</v>
+      </c>
+      <c r="D13" s="15" t="n">
+        <v>39</v>
+      </c>
+      <c r="E13" s="15" t="n">
+        <v>0.35039640768</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="15" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="15" t="n">
+        <v>93</v>
+      </c>
+      <c r="D14" s="15" t="n">
+        <v>160</v>
+      </c>
+      <c r="E14" s="15" t="n">
+        <v>0.58685784336</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="15" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="15" t="n">
+        <v>122</v>
+      </c>
+      <c r="D15" s="15" t="n">
+        <v>54</v>
+      </c>
+      <c r="E15" s="15" t="n">
+        <v>0.24311220636</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="15" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="15" t="n">
+        <v>145</v>
+      </c>
+      <c r="D16" s="15" t="n">
+        <v>181</v>
+      </c>
+      <c r="E16" s="15" t="n">
+        <v>0.2981113254</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="15" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="15" t="n">
+        <v>190</v>
+      </c>
+      <c r="D17" s="15" t="n">
+        <v>64</v>
+      </c>
+      <c r="E17" s="15" t="n">
+        <v>1.3821818328</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="15" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="15" t="n">
+        <v>85</v>
+      </c>
+      <c r="D18" s="15" t="n">
+        <v>530</v>
+      </c>
+      <c r="E18" s="15" t="n">
+        <v>1.3821818328</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="15" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="15" t="n">
+        <v>87</v>
+      </c>
+      <c r="D19" s="15" t="n">
+        <v>38.5</v>
+      </c>
+      <c r="E19" s="15" t="n">
+        <v>0.65778210996</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="15" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="15" t="n">
+        <v>120</v>
+      </c>
+      <c r="E20" s="15" t="n">
+        <v>1.7063034312</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="15" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="15" t="n">
+        <v>150</v>
+      </c>
+      <c r="D21" s="15" t="n">
+        <v>10</v>
+      </c>
+      <c r="E21" s="15" t="n">
+        <v>0.073060043712</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="15" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="15" t="n">
+        <v>221</v>
+      </c>
+      <c r="D22" s="15" t="n">
+        <v>13</v>
+      </c>
+      <c r="E22" s="0"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="15" t="n">
+        <v>2018</v>
+      </c>
+      <c r="B23" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="15" t="n">
+        <v>368</v>
+      </c>
+      <c r="D23" s="15" t="n">
+        <v>375</v>
+      </c>
+      <c r="E23" s="15" t="n">
+        <v>0.44133636708</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
filled in cn in 2018 17 flux xlsx to match n2
</commit_message>
<xml_diff>
--- a/data/flux/2017_2018_flux+rate_MED.xlsx
+++ b/data/flux/2017_2018_flux+rate_MED.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="2017 P2 rates not ctl sub" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="205">
   <si>
     <t xml:space="preserve">P2 +Particles</t>
   </si>
@@ -571,9 +571,15 @@
     <t xml:space="preserve">Keil 3-36</t>
   </si>
   <si>
+    <t xml:space="preserve">lots of pteropods</t>
+  </si>
+  <si>
     <t xml:space="preserve">Keil 4-34</t>
   </si>
   <si>
+    <t xml:space="preserve">pteropod</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kel 4-31</t>
   </si>
   <si>
@@ -586,7 +592,13 @@
     <t xml:space="preserve">Keil 1-30</t>
   </si>
   <si>
+    <t xml:space="preserve">no zoops</t>
+  </si>
+  <si>
     <t xml:space="preserve">Keil 2-33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lanternfish</t>
   </si>
   <si>
     <t xml:space="preserve">To copy into 2018_fluxes.xlsx for plotting with maplotlib in jupyter notebooks</t>
@@ -1075,7 +1087,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart117.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1087,10 +1099,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.101492537313433"/>
-          <c:y val="0.164556002123303"/>
-          <c:w val="0.855909640984268"/>
-          <c:h val="0.784712216576932"/>
+          <c:x val="0.101482104718141"/>
+          <c:y val="0.16456848172304"/>
+          <c:w val="0.855866934179018"/>
+          <c:h val="0.784620051569847"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1246,11 +1258,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="29945789"/>
-        <c:axId val="46551912"/>
+        <c:axId val="97603809"/>
+        <c:axId val="10473286"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="29945789"/>
+        <c:axId val="97603809"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1316,13 +1328,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46551912"/>
+        <c:crossAx val="10473286"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="46551912"/>
+        <c:axId val="10473286"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="1000"/>
@@ -1355,7 +1367,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29945789"/>
+        <c:crossAx val="97603809"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1382,7 +1394,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart118.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1394,10 +1406,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.101510128913444"/>
-          <c:y val="0.164579876301101"/>
-          <c:w val="0.855911602209945"/>
-          <c:h val="0.784658319505204"/>
+          <c:x val="0.101498878791455"/>
+          <c:y val="0.164592290865203"/>
+          <c:w val="0.855836185530509"/>
+          <c:h val="0.784566644037113"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1549,11 +1561,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="7253022"/>
-        <c:axId val="86235472"/>
+        <c:axId val="33118937"/>
+        <c:axId val="39967880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="7253022"/>
+        <c:axId val="33118937"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1620,13 +1632,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86235472"/>
+        <c:crossAx val="39967880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="86235472"/>
+        <c:axId val="39967880"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="300"/>
@@ -1659,7 +1671,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7253022"/>
+        <c:crossAx val="33118937"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1686,7 +1698,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart119.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1698,10 +1710,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.206261510128913"/>
-          <c:y val="0.164482937301059"/>
-          <c:w val="0.731123388581952"/>
-          <c:h val="0.784736101858021"/>
+          <c:x val="0.206240614049725"/>
+          <c:y val="0.164495114006515"/>
+          <c:w val="0.731075143222649"/>
+          <c:h val="0.784646135623334"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1853,11 +1865,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="57755841"/>
-        <c:axId val="16720403"/>
+        <c:axId val="85280306"/>
+        <c:axId val="54146051"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="57755841"/>
+        <c:axId val="85280306"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -1925,12 +1937,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16720403"/>
+        <c:crossAx val="54146051"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="16720403"/>
+        <c:axId val="54146051"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="1000"/>
@@ -1997,7 +2009,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57755841"/>
+        <c:crossAx val="85280306"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2024,7 +2036,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart120.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2036,10 +2048,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.206365809922295"/>
-          <c:y val="0.196842554401934"/>
-          <c:w val="0.731171548117155"/>
-          <c:h val="0.752382306926468"/>
+          <c:x val="0.206335213916314"/>
+          <c:y val="0.196856553587938"/>
+          <c:w val="0.731135401974612"/>
+          <c:h val="0.752293577981651"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2325,11 +2337,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="31068688"/>
-        <c:axId val="21719439"/>
+        <c:axId val="27153068"/>
+        <c:axId val="47174141"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="31068688"/>
+        <c:axId val="27153068"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -2367,8 +2379,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.170277943813509"/>
-              <c:y val="0.00533352296970559"/>
+              <c:x val="0.170310296191819"/>
+              <c:y val="0.00533390228291018"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2405,13 +2417,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="21719439"/>
+        <c:crossAx val="47174141"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="21719439"/>
+        <c:axId val="47174141"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="300"/>
@@ -2478,7 +2490,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31068688"/>
+        <c:crossAx val="27153068"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2505,7 +2517,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart121.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2517,10 +2529,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.206327372764787"/>
-          <c:y val="0.164554147209251"/>
-          <c:w val="0.731149180942854"/>
-          <c:h val="0.784523015343562"/>
+          <c:x val="0.206330768113838"/>
+          <c:y val="0.164572445235183"/>
+          <c:w val="0.731135956633271"/>
+          <c:h val="0.784387857222284"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2672,11 +2684,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="86328198"/>
-        <c:axId val="69781040"/>
+        <c:axId val="1578169"/>
+        <c:axId val="53562164"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86328198"/>
+        <c:axId val="1578169"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -2744,12 +2756,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69781040"/>
+        <c:crossAx val="53562164"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="69781040"/>
+        <c:axId val="53562164"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="1000"/>
@@ -2816,7 +2828,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86328198"/>
+        <c:crossAx val="1578169"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2843,7 +2855,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart122.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2855,10 +2867,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.101513599635826"/>
-          <c:y val="0.164545274681791"/>
-          <c:w val="0.856094230112666"/>
-          <c:h val="0.784739167710875"/>
+          <c:x val="0.101488560139667"/>
+          <c:y val="0.164556127160005"/>
+          <c:w val="0.8560599099513"/>
+          <c:h val="0.784659015960955"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2999,11 +3011,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="40717422"/>
-        <c:axId val="4436703"/>
+        <c:axId val="71702069"/>
+        <c:axId val="6293587"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="40717422"/>
+        <c:axId val="71702069"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3035,13 +3047,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4436703"/>
+        <c:crossAx val="6293587"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="4436703"/>
+        <c:axId val="6293587"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="1000"/>
@@ -3074,7 +3086,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40717422"/>
+        <c:crossAx val="71702069"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="200"/>
@@ -3102,7 +3114,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart123.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3114,10 +3126,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.101556463185782"/>
-          <c:y val="0.164491218478781"/>
-          <c:w val="0.856054752180152"/>
-          <c:h val="0.784801476115629"/>
+          <c:x val="0.101540067867398"/>
+          <c:y val="0.164502460360853"/>
+          <c:w val="0.855999303924128"/>
+          <c:h val="0.784718425369054"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3415,11 +3427,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="96217218"/>
-        <c:axId val="61252130"/>
+        <c:axId val="14761127"/>
+        <c:axId val="90923199"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="96217218"/>
+        <c:axId val="14761127"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -3452,13 +3464,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61252130"/>
+        <c:crossAx val="90923199"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61252130"/>
+        <c:axId val="90923199"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="300"/>
@@ -3491,7 +3503,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96217218"/>
+        <c:crossAx val="14761127"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="50"/>
@@ -3519,7 +3531,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart124.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3531,10 +3543,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.206279378088466"/>
-          <c:y val="0.196911998892197"/>
-          <c:w val="0.73116789200916"/>
-          <c:h val="0.752406009831752"/>
+          <c:x val="0.206271178351549"/>
+          <c:y val="0.196925633568758"/>
+          <c:w val="0.731112489858254"/>
+          <c:h val="0.75231962332087"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3680,11 +3692,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="2900974"/>
-        <c:axId val="20471881"/>
+        <c:axId val="90351545"/>
+        <c:axId val="45127834"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2900974"/>
+        <c:axId val="90351545"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -3718,13 +3730,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20471881"/>
+        <c:crossAx val="45127834"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="20471881"/>
+        <c:axId val="45127834"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="300"/>
@@ -3757,7 +3769,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2900974"/>
+        <c:crossAx val="90351545"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3784,7 +3796,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart125.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart25.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3796,10 +3808,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.206320571924901"/>
-          <c:y val="0.164532019704433"/>
-          <c:w val="0.731141845393198"/>
-          <c:h val="0.784691170898067"/>
+          <c:x val="0.206328133643102"/>
+          <c:y val="0.16454448991966"/>
+          <c:w val="0.731109636021684"/>
+          <c:h val="0.784599060178869"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -3951,11 +3963,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="30601671"/>
-        <c:axId val="37286723"/>
+        <c:axId val="90862957"/>
+        <c:axId val="77554160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="30601671"/>
+        <c:axId val="90862957"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4023,13 +4035,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37286723"/>
+        <c:crossAx val="77554160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="37286723"/>
+        <c:axId val="77554160"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="1000"/>
@@ -4096,7 +4108,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30601671"/>
+        <c:crossAx val="90862957"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4123,7 +4135,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart126.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart26.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4135,10 +4147,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.206356116673922"/>
-          <c:y val="0.196853171523319"/>
-          <c:w val="0.73120218919087"/>
-          <c:h val="0.75234601001905"/>
+          <c:x val="0.206321022727273"/>
+          <c:y val="0.196867061812024"/>
+          <c:w val="0.731178977272727"/>
+          <c:h val="0.752257973468812"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -4356,11 +4368,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="61038267"/>
-        <c:axId val="46880951"/>
+        <c:axId val="24096534"/>
+        <c:axId val="67520418"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61038267"/>
+        <c:axId val="24096534"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="20"/>
@@ -4394,13 +4406,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46880951"/>
+        <c:crossAx val="67520418"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="46880951"/>
+        <c:axId val="67520418"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="300"/>
@@ -4433,7 +4445,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61038267"/>
+        <c:crossAx val="24096534"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4460,7 +4472,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart127.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4472,10 +4484,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.101579986833443"/>
-          <c:y val="0.164486692015209"/>
-          <c:w val="0.855957867017775"/>
-          <c:h val="0.784714828897338"/>
+          <c:x val="0.101590874213515"/>
+          <c:y val="0.164499201460187"/>
+          <c:w val="0.855900557573277"/>
+          <c:h val="0.784622404745608"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -4619,11 +4631,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="23013407"/>
-        <c:axId val="74767458"/>
+        <c:axId val="96063075"/>
+        <c:axId val="24988268"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="23013407"/>
+        <c:axId val="96063075"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -4660,8 +4672,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.232455562870309"/>
-              <c:y val="0.0248669201520913"/>
+              <c:x val="0.232441557112896"/>
+              <c:y val="0.0249448627272036"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -4698,13 +4710,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74767458"/>
+        <c:crossAx val="24988268"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="74767458"/>
+        <c:axId val="24988268"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="700"/>
@@ -4737,7 +4749,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23013407"/>
+        <c:crossAx val="96063075"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4764,7 +4776,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart128.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4776,10 +4788,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.101517107811491"/>
-          <c:y val="0.164556002123303"/>
-          <c:w val="0.855874757908328"/>
-          <c:h val="0.784712216576932"/>
+          <c:x val="0.101520259525475"/>
+          <c:y val="0.16456848172304"/>
+          <c:w val="0.855797977227912"/>
+          <c:h val="0.784620051569847"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -4935,11 +4947,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="7452326"/>
-        <c:axId val="64146388"/>
+        <c:axId val="79829533"/>
+        <c:axId val="28286821"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="7452326"/>
+        <c:axId val="79829533"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5005,13 +5017,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64146388"/>
+        <c:crossAx val="28286821"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64146388"/>
+        <c:axId val="28286821"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="1000"/>
@@ -5044,7 +5056,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7452326"/>
+        <c:crossAx val="79829533"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5071,7 +5083,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart129.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5083,10 +5095,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.101532567049808"/>
-          <c:y val="0.164579876301101"/>
-          <c:w val="0.855879752431476"/>
-          <c:h val="0.784658319505204"/>
+          <c:x val="0.10151250727167"/>
+          <c:y val="0.164592290865203"/>
+          <c:w val="0.855846422338569"/>
+          <c:h val="0.784566644037113"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -5238,11 +5250,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="96429784"/>
-        <c:axId val="25192437"/>
+        <c:axId val="30231324"/>
+        <c:axId val="15290303"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="96429784"/>
+        <c:axId val="30231324"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -5309,13 +5321,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25192437"/>
+        <c:crossAx val="15290303"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="25192437"/>
+        <c:axId val="15290303"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="300"/>
@@ -5348,7 +5360,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96429784"/>
+        <c:crossAx val="30231324"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5375,7 +5387,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart130.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5387,10 +5399,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.206313712594541"/>
-          <c:y val="0.164482937301059"/>
-          <c:w val="0.731141072015784"/>
-          <c:h val="0.784736101858021"/>
+          <c:x val="0.206296234495801"/>
+          <c:y val="0.164495114006515"/>
+          <c:w val="0.731075143222649"/>
+          <c:h val="0.784646135623334"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -5542,11 +5554,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="20680081"/>
-        <c:axId val="61653272"/>
+        <c:axId val="15058329"/>
+        <c:axId val="55445130"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="20680081"/>
+        <c:axId val="15058329"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.5"/>
@@ -5614,12 +5626,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61653272"/>
+        <c:crossAx val="55445130"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61653272"/>
+        <c:axId val="55445130"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="1000"/>
@@ -5686,7 +5698,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20680081"/>
+        <c:crossAx val="15058329"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5713,7 +5725,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart131.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5725,10 +5737,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.206327372764787"/>
-          <c:y val="0.164554147209251"/>
-          <c:w val="0.731149180942854"/>
-          <c:h val="0.784523015343562"/>
+          <c:x val="0.206330768113838"/>
+          <c:y val="0.164572445235183"/>
+          <c:w val="0.731135956633271"/>
+          <c:h val="0.784387857222284"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -5880,11 +5892,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="46193895"/>
-        <c:axId val="29383154"/>
+        <c:axId val="16739977"/>
+        <c:axId val="29933677"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="46193895"/>
+        <c:axId val="16739977"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -5952,12 +5964,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29383154"/>
+        <c:crossAx val="29933677"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="29383154"/>
+        <c:axId val="29933677"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="1000"/>
@@ -6024,7 +6036,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46193895"/>
+        <c:crossAx val="16739977"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6051,7 +6063,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart132.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart32.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -6063,10 +6075,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.101530931648739"/>
-          <c:y val="0.164545274681791"/>
-          <c:w val="0.856069660235615"/>
-          <c:h val="0.784739167710875"/>
+          <c:x val="0.101544437251457"/>
+          <c:y val="0.164556127160005"/>
+          <c:w val="0.856052899287894"/>
+          <c:h val="0.784659015960955"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -6207,11 +6219,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="11819657"/>
-        <c:axId val="57343140"/>
+        <c:axId val="64542862"/>
+        <c:axId val="23105639"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="11819657"/>
+        <c:axId val="64542862"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6243,13 +6255,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57343140"/>
+        <c:crossAx val="23105639"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="57343140"/>
+        <c:axId val="23105639"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="1000"/>
@@ -6282,7 +6294,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11819657"/>
+        <c:crossAx val="64542862"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="200"/>
@@ -6310,7 +6322,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart133.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart33.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -6322,10 +6334,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.101562068775184"/>
-          <c:y val="0.164491218478781"/>
-          <c:w val="0.855991610089971"/>
-          <c:h val="0.784801476115629"/>
+          <c:x val="0.101550454000343"/>
+          <c:y val="0.164502460360853"/>
+          <c:w val="0.855961966763748"/>
+          <c:h val="0.784718425369054"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -6623,11 +6635,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="16658294"/>
-        <c:axId val="59529950"/>
+        <c:axId val="15071915"/>
+        <c:axId val="14487281"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="16658294"/>
+        <c:axId val="15071915"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -6660,13 +6672,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59529950"/>
+        <c:crossAx val="14487281"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="59529950"/>
+        <c:axId val="14487281"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="300"/>
@@ -6699,7 +6711,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16658294"/>
+        <c:crossAx val="15071915"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="50"/>
@@ -6727,7 +6739,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart134.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart34.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -6739,10 +6751,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.206334357877856"/>
-          <c:y val="0.164532019704433"/>
-          <c:w val="0.731190698917546"/>
-          <c:h val="0.784691170898067"/>
+          <c:x val="0.206328133643102"/>
+          <c:y val="0.16454448991966"/>
+          <c:w val="0.731164951875207"/>
+          <c:h val="0.784599060178869"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -6894,11 +6906,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="44147987"/>
-        <c:axId val="10327543"/>
+        <c:axId val="65972070"/>
+        <c:axId val="77468680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="44147987"/>
+        <c:axId val="65972070"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -6966,13 +6978,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10327543"/>
+        <c:crossAx val="77468680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.2"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="10327543"/>
+        <c:axId val="77468680"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="1000"/>
@@ -7039,7 +7051,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44147987"/>
+        <c:crossAx val="65972070"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7066,7 +7078,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart135.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart35.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -7194,11 +7206,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="17377496"/>
-        <c:axId val="36084150"/>
+        <c:axId val="87572247"/>
+        <c:axId val="68603954"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="17377496"/>
+        <c:axId val="87572247"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7254,12 +7266,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36084150"/>
+        <c:crossAx val="68603954"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="36084150"/>
+        <c:axId val="68603954"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -7315,7 +7327,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17377496"/>
+        <c:crossAx val="87572247"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7342,7 +7354,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart136.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart36.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -7484,11 +7496,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="16668324"/>
-        <c:axId val="96886109"/>
+        <c:axId val="35294344"/>
+        <c:axId val="29840827"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="16668324"/>
+        <c:axId val="35294344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7544,12 +7556,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96886109"/>
+        <c:crossAx val="29840827"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="96886109"/>
+        <c:axId val="29840827"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="400"/>
@@ -7606,7 +7618,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16668324"/>
+        <c:crossAx val="35294344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7633,7 +7645,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart137.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart37.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -7856,11 +7868,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="69946572"/>
-        <c:axId val="20473058"/>
+        <c:axId val="97056200"/>
+        <c:axId val="73526956"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="69946572"/>
+        <c:axId val="97056200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7916,12 +7928,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="20473058"/>
+        <c:crossAx val="73526956"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="20473058"/>
+        <c:axId val="73526956"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -7977,7 +7989,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69946572"/>
+        <c:crossAx val="97056200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8004,7 +8016,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart138.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart38.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -8209,11 +8221,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="96359597"/>
-        <c:axId val="31500163"/>
+        <c:axId val="84897435"/>
+        <c:axId val="13862497"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="96359597"/>
+        <c:axId val="84897435"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8269,12 +8281,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31500163"/>
+        <c:crossAx val="13862497"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="31500163"/>
+        <c:axId val="13862497"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="400"/>
@@ -8331,7 +8343,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96359597"/>
+        <c:crossAx val="84897435"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8358,7 +8370,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart139.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart39.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -8518,11 +8530,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="27769924"/>
-        <c:axId val="30594039"/>
+        <c:axId val="87709801"/>
+        <c:axId val="44230978"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="27769924"/>
+        <c:axId val="87709801"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8578,12 +8590,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30594039"/>
+        <c:crossAx val="44230978"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="30594039"/>
+        <c:axId val="44230978"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="400"/>
@@ -8640,7 +8652,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27769924"/>
+        <c:crossAx val="87709801"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8678,9 +8690,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>766080</xdr:colOff>
+      <xdr:colOff>765720</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>133920</xdr:rowOff>
+      <xdr:rowOff>133560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8688,8 +8700,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1626480" y="7784640"/>
-        <a:ext cx="4461840" cy="4746960"/>
+        <a:off x="1888200" y="7784640"/>
+        <a:ext cx="5562000" cy="4746600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8708,9 +8720,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>970920</xdr:colOff>
+      <xdr:colOff>970560</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>54000</xdr:rowOff>
+      <xdr:rowOff>53640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8718,8 +8730,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5250240" y="7679160"/>
-        <a:ext cx="4886640" cy="4772520"/>
+        <a:off x="6381000" y="7679160"/>
+        <a:ext cx="6100200" cy="4772160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8738,9 +8750,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>1672200</xdr:colOff>
+      <xdr:colOff>1671840</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>144360</xdr:rowOff>
+      <xdr:rowOff>144000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8748,8 +8760,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10478880" y="7679160"/>
-        <a:ext cx="5473080" cy="4862880"/>
+        <a:off x="13132440" y="7679160"/>
+        <a:ext cx="6472080" cy="4862520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8768,9 +8780,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>132120</xdr:colOff>
+      <xdr:colOff>131760</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>18720</xdr:rowOff>
+      <xdr:rowOff>18360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8778,8 +8790,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="44038800" y="5068440"/>
-        <a:ext cx="4817880" cy="5061960"/>
+        <a:off x="55209240" y="5068440"/>
+        <a:ext cx="6125400" cy="5061600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8798,9 +8810,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>576720</xdr:colOff>
+      <xdr:colOff>576360</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>191160</xdr:rowOff>
+      <xdr:rowOff>190800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8808,8 +8820,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="15659640" y="7636680"/>
-        <a:ext cx="5757480" cy="3237480"/>
+        <a:off x="19312560" y="7636680"/>
+        <a:ext cx="7437600" cy="3237120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8828,9 +8840,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>432720</xdr:colOff>
+      <xdr:colOff>432360</xdr:colOff>
       <xdr:row>80</xdr:row>
-      <xdr:rowOff>124560</xdr:rowOff>
+      <xdr:rowOff>124200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8838,8 +8850,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1943280" y="10492920"/>
-        <a:ext cx="6326280" cy="5458320"/>
+        <a:off x="2438640" y="10492920"/>
+        <a:ext cx="7835400" cy="5457960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8858,9 +8870,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>646560</xdr:colOff>
+      <xdr:colOff>646200</xdr:colOff>
       <xdr:row>80</xdr:row>
-      <xdr:rowOff>124200</xdr:rowOff>
+      <xdr:rowOff>123840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8868,8 +8880,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7286400" y="10683360"/>
-        <a:ext cx="6522120" cy="5267520"/>
+        <a:off x="8901000" y="10683360"/>
+        <a:ext cx="8274600" cy="5267160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8888,9 +8900,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>574560</xdr:colOff>
+      <xdr:colOff>574200</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>7200</xdr:rowOff>
+      <xdr:rowOff>6840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8898,8 +8910,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="43325640" y="4538520"/>
-        <a:ext cx="5973480" cy="5199120"/>
+        <a:off x="54234360" y="4538520"/>
+        <a:ext cx="7542720" cy="5198760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8918,9 +8930,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>1013760</xdr:colOff>
+      <xdr:colOff>1013400</xdr:colOff>
       <xdr:row>77</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>177840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8928,8 +8940,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="14279760" y="10683360"/>
-        <a:ext cx="5387760" cy="4749840"/>
+        <a:off x="17932680" y="10683360"/>
+        <a:ext cx="6507720" cy="4749480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8948,9 +8960,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>43</xdr:col>
-      <xdr:colOff>690120</xdr:colOff>
+      <xdr:colOff>689760</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>86760</xdr:rowOff>
+      <xdr:rowOff>86400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8958,8 +8970,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="49745520" y="4334400"/>
-        <a:ext cx="5788080" cy="5101920"/>
+        <a:off x="62485560" y="4334400"/>
+        <a:ext cx="7095960" cy="5101560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -8983,9 +8995,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>136440</xdr:colOff>
+      <xdr:colOff>136080</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -8993,8 +9005,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3846600" y="5970240"/>
-        <a:ext cx="5468040" cy="4733640"/>
+        <a:off x="4631400" y="5970240"/>
+        <a:ext cx="7037280" cy="4733280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9018,9 +9030,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>441720</xdr:colOff>
+      <xdr:colOff>441360</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>67320</xdr:rowOff>
+      <xdr:rowOff>66960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9028,8 +9040,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1680480" y="3014640"/>
-        <a:ext cx="4460760" cy="4746960"/>
+        <a:off x="1942200" y="3014640"/>
+        <a:ext cx="5659200" cy="4746600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9048,9 +9060,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>631800</xdr:colOff>
+      <xdr:colOff>631440</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>61920</xdr:rowOff>
+      <xdr:rowOff>61560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9058,8 +9070,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6532200" y="3555000"/>
-        <a:ext cx="4885560" cy="4772520"/>
+        <a:off x="7992720" y="3555000"/>
+        <a:ext cx="6188040" cy="4772160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9078,9 +9090,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>1672560</xdr:colOff>
+      <xdr:colOff>1672200</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>152280</xdr:rowOff>
+      <xdr:rowOff>151920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9088,8 +9100,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="12413160" y="3555000"/>
-        <a:ext cx="5473440" cy="4862880"/>
+        <a:off x="15566760" y="3555000"/>
+        <a:ext cx="6472080" cy="4862520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9108,9 +9120,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>576720</xdr:colOff>
+      <xdr:colOff>576360</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>8280</xdr:rowOff>
+      <xdr:rowOff>7920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9118,8 +9130,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="17593920" y="3512520"/>
-        <a:ext cx="5757480" cy="3237480"/>
+        <a:off x="21746520" y="3512520"/>
+        <a:ext cx="7437600" cy="3237120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9138,9 +9150,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>633600</xdr:colOff>
+      <xdr:colOff>633240</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9148,8 +9160,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2047680" y="6369120"/>
-        <a:ext cx="6325200" cy="5458320"/>
+        <a:off x="2571120" y="6369120"/>
+        <a:ext cx="7785000" cy="5457960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9168,9 +9180,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
+      <xdr:colOff>136800</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9178,8 +9190,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8711640" y="6559920"/>
-        <a:ext cx="6521760" cy="5267520"/>
+        <a:off x="10695240" y="6559920"/>
+        <a:ext cx="8404920" cy="5267160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9198,9 +9210,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>1013760</xdr:colOff>
+      <xdr:colOff>1013400</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>186480</xdr:rowOff>
+      <xdr:rowOff>186120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9208,8 +9220,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="16214040" y="6559920"/>
-        <a:ext cx="5387400" cy="4749840"/>
+        <a:off x="20366640" y="6559920"/>
+        <a:ext cx="6507720" cy="4749480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9233,9 +9245,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>254160</xdr:colOff>
+      <xdr:colOff>253800</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>65160</xdr:rowOff>
+      <xdr:rowOff>64800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9243,8 +9255,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8112600" y="364680"/>
-        <a:ext cx="3520440" cy="4038480"/>
+        <a:off x="9981360" y="364680"/>
+        <a:ext cx="4558320" cy="4038120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9268,9 +9280,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>438120</xdr:colOff>
+      <xdr:colOff>437760</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>151920</xdr:rowOff>
+      <xdr:rowOff>151560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9278,8 +9290,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10267200" y="4659120"/>
-        <a:ext cx="3195720" cy="4123080"/>
+        <a:off x="12759120" y="4659120"/>
+        <a:ext cx="4025880" cy="4122720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9298,9 +9310,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>446040</xdr:colOff>
+      <xdr:colOff>445680</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>159840</xdr:rowOff>
+      <xdr:rowOff>159480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9308,8 +9320,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10275120" y="467640"/>
-        <a:ext cx="3195720" cy="4123080"/>
+        <a:off x="12767040" y="467640"/>
+        <a:ext cx="4025880" cy="4122720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9328,9 +9340,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>494640</xdr:colOff>
+      <xdr:colOff>494280</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>164160</xdr:rowOff>
+      <xdr:rowOff>163800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9338,8 +9350,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7067160" y="467640"/>
-        <a:ext cx="3196080" cy="4127400"/>
+        <a:off x="8728200" y="467640"/>
+        <a:ext cx="4026600" cy="4127040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9358,9 +9370,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>535320</xdr:colOff>
+      <xdr:colOff>534960</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>181800</xdr:rowOff>
+      <xdr:rowOff>181440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -9368,8 +9380,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7108200" y="4689000"/>
-        <a:ext cx="3195720" cy="4123080"/>
+        <a:off x="8769240" y="4689000"/>
+        <a:ext cx="4026240" cy="4122720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -9393,31 +9405,31 @@
       <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="19.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="14" style="0" width="28.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="30.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="0" width="18.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="21.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="39.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="23" style="0" width="13.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="23" style="0" width="13.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="23.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="23.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="31" style="0" width="13.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="31" style="0" width="13.19"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11763,16 +11775,16 @@
       <selection pane="topLeft" activeCell="T24" activeCellId="0" sqref="T24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="1" style="0" width="13.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="1" style="0" width="13.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="11" style="0" width="21.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="30.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="26.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="0" width="13.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="0" width="13.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="30.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="19" style="0" width="13.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="19" style="0" width="13.19"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13058,28 +13070,28 @@
   </sheetPr>
   <dimension ref="A1:AS29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA4" activeCellId="0" sqref="AA4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="X1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AB8" activeCellId="0" sqref="AB8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="13.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="13.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="13.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="8" style="0" width="19.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="13.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="8" style="0" width="19.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="14" style="0" width="28.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="30.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="0" width="18.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="21.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="39.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="23" style="0" width="13.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="23" style="0" width="13.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="23.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="23.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="30" style="0" width="13.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="30" style="0" width="13.19"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13596,6 +13608,9 @@
         <f aca="false">N8/$AD$2</f>
         <v>0.163540598537405</v>
       </c>
+      <c r="V8" s="0" t="s">
+        <v>171</v>
+      </c>
       <c r="W8" s="0" t="n">
         <v>2018</v>
       </c>
@@ -13637,7 +13652,7 @@
         <v>87</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>40</v>
@@ -13671,6 +13686,9 @@
         <f aca="false">N9/$AD$2</f>
         <v>0.0778291809494656</v>
       </c>
+      <c r="V9" s="0" t="s">
+        <v>173</v>
+      </c>
       <c r="W9" s="0" t="n">
         <v>2018</v>
       </c>
@@ -13698,7 +13716,7 @@
         <v>35</v>
       </c>
       <c r="AF9" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AS9" s="5" t="s">
         <v>55</v>
@@ -13712,7 +13730,7 @@
         <v>121</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>1</v>
@@ -13741,7 +13759,7 @@
         <v>0.201890863996947</v>
       </c>
       <c r="V10" s="26" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="W10" s="0" t="n">
         <v>2018</v>
@@ -13760,7 +13778,7 @@
         <v>15</v>
       </c>
       <c r="AF10" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="AS10" s="5" t="s">
         <v>58</v>
@@ -13774,7 +13792,7 @@
         <v>150</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>40</v>
@@ -13808,6 +13826,9 @@
         <f aca="false">N11/$AD$2</f>
         <v>0.162546630155725</v>
       </c>
+      <c r="V11" s="0" t="s">
+        <v>178</v>
+      </c>
       <c r="W11" s="0" t="n">
         <v>2018</v>
       </c>
@@ -13835,7 +13856,7 @@
         <v>15</v>
       </c>
       <c r="AF11" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="AS11" s="5" t="s">
         <v>60</v>
@@ -13849,7 +13870,7 @@
         <v>221</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>40</v>
@@ -13883,6 +13904,9 @@
         <f aca="false">N12/$AD$2</f>
         <v>0.413103197931298</v>
       </c>
+      <c r="V12" s="0" t="s">
+        <v>178</v>
+      </c>
       <c r="W12" s="0" t="n">
         <v>2018</v>
       </c>
@@ -13910,7 +13934,7 @@
         <v>35</v>
       </c>
       <c r="AF12" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13921,7 +13945,7 @@
         <v>368</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>53</v>
@@ -13955,6 +13979,9 @@
         <f aca="false">N13/$AD$2</f>
         <v>0.0522191884712977</v>
       </c>
+      <c r="V13" s="0" t="s">
+        <v>180</v>
+      </c>
       <c r="W13" s="0" t="n">
         <v>2018</v>
       </c>
@@ -13982,12 +14009,12 @@
         <v>50</v>
       </c>
       <c r="AF13" s="0" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="X15" s="0" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14001,10 +14028,10 @@
         <v>18</v>
       </c>
       <c r="Z16" s="0" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="AA16" s="0" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14112,7 +14139,7 @@
         <v>43</v>
       </c>
       <c r="X22" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="Y22" s="0" t="n">
         <v>87</v>
@@ -14132,13 +14159,13 @@
         <v>43</v>
       </c>
       <c r="X23" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="Y23" s="0" t="n">
         <v>121</v>
       </c>
       <c r="Z23" s="0" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="AB23" s="0" t="n">
         <v>4.2</v>
@@ -14149,7 +14176,7 @@
         <v>43</v>
       </c>
       <c r="X24" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="Y24" s="0" t="n">
         <v>150</v>
@@ -14169,7 +14196,7 @@
         <v>43</v>
       </c>
       <c r="X25" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="Y25" s="0" t="n">
         <v>221</v>
@@ -14189,7 +14216,7 @@
         <v>43</v>
       </c>
       <c r="X26" s="0" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="Y26" s="0" t="n">
         <v>368</v>
@@ -14206,7 +14233,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="Z27" s="0" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="AA27" s="0" t="n">
         <f aca="false">AVERAGE(AA17:AA26)</f>
@@ -14266,14 +14293,14 @@
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1016" min="1" style="27" width="10.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="27" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B1" s="27" t="s">
         <v>81</v>
@@ -14282,16 +14309,16 @@
         <v>18</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="F1" s="27" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="G1" s="27" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14852,23 +14879,23 @@
   </sheetPr>
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M48" activeCellId="0" sqref="M48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D1" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>81</v>
@@ -14883,7 +14910,7 @@
         <v>36</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14972,7 +14999,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F7" s="0" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15096,12 +15123,12 @@
         <v>12</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>81</v>
@@ -15116,7 +15143,7 @@
         <v>36</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15247,7 +15274,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F25" s="0" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15441,7 +15468,7 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="D36" s="0" t="n">
         <f aca="false">AVERAGE(E26:E27)</f>
@@ -15450,7 +15477,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="E38" s="0" t="n">
         <f aca="false">AVERAGE(E3:E13,E26:E34)</f>
@@ -15480,7 +15507,7 @@
       <selection pane="topLeft" activeCell="O28" activeCellId="0" sqref="O28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="1" style="28" width="10.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="28" width="15.2"/>
@@ -15489,13 +15516,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="28" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="K1" s="28" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15974,7 +16001,7 @@
         <v>43</v>
       </c>
       <c r="L31" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="M31" s="0" t="n">
         <v>38.5</v>
@@ -15992,7 +16019,7 @@
         <v>43</v>
       </c>
       <c r="L32" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="M32" s="0"/>
       <c r="N32" s="0"/>
@@ -16006,7 +16033,7 @@
         <v>43</v>
       </c>
       <c r="L33" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="M33" s="0" t="n">
         <v>10</v>
@@ -16024,7 +16051,7 @@
         <v>43</v>
       </c>
       <c r="L34" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="M34" s="0" t="n">
         <v>13</v>
@@ -16042,7 +16069,7 @@
         <v>43</v>
       </c>
       <c r="L35" s="0" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="M35" s="0" t="n">
         <v>375</v>
@@ -16105,7 +16132,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K40" s="28" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="M40" s="29" t="s">
         <v>98</v>
@@ -16167,20 +16194,20 @@
       <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="31" width="15.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="31" width="15.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="31" width="13.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="31" width="13.19"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="4" style="31" width="10.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>18</v>
@@ -16456,7 +16483,7 @@
         <v>42</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C9" s="3" t="n">
         <v>100</v>
@@ -16494,7 +16521,7 @@
         <v>46</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C10" s="3" t="n">
         <v>100</v>
@@ -16532,7 +16559,7 @@
         <v>48</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C11" s="3" t="n">
         <v>113</v>
@@ -16570,7 +16597,7 @@
         <v>51</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C12" s="3" t="n">
         <v>120</v>
@@ -16608,7 +16635,7 @@
         <v>54</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C13" s="3" t="n">
         <v>120</v>
@@ -16646,7 +16673,7 @@
         <v>57</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C14" s="3" t="n">
         <v>140</v>
@@ -16680,7 +16707,7 @@
         <v>59</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C15" s="3" t="n">
         <v>150</v>
@@ -16718,7 +16745,7 @@
         <v>63</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C16" s="3" t="n">
         <v>150</v>
@@ -16756,7 +16783,7 @@
         <v>65</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C17" s="3" t="n">
         <v>179</v>
@@ -16794,7 +16821,7 @@
         <v>66</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C18" s="3" t="n">
         <v>180</v>

</xml_diff>